<commit_message>
add getQ and can learn many times if the time is permitted
</commit_message>
<xml_diff>
--- a/Q2_2.xlsx
+++ b/Q2_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\学习资料\大二下课程\数学建模\正式赛\P1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C627B8-9495-41E9-BE60-3A5D36D7B895}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9993776E-D0F4-4635-A1C9-29FFAD0FC347}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A7902C27-006F-4924-B8BD-1931EA3404E5}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="26">
   <si>
     <t>状态</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -126,6 +126,10 @@
   </si>
   <si>
     <t>corr+ 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态编号</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -490,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01C87B4-D936-4DBF-AB49-DF2BE20DF922}">
-  <dimension ref="B1:I29"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -504,7 +508,7 @@
     <col min="7" max="7" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +516,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -529,7 +536,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -549,7 +559,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
       <c r="B4">
         <v>0</v>
       </c>
@@ -569,7 +582,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
       <c r="B5">
         <v>0</v>
       </c>
@@ -589,7 +605,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
       <c r="B6">
         <v>0</v>
       </c>
@@ -606,7 +625,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
       <c r="B7">
         <v>0</v>
       </c>
@@ -623,7 +645,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
       <c r="B8">
         <v>0</v>
       </c>
@@ -640,7 +665,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
       <c r="B9">
         <v>0</v>
       </c>
@@ -657,7 +685,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
       <c r="B10">
         <v>0</v>
       </c>
@@ -674,7 +705,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
       <c r="B11">
         <v>0</v>
       </c>
@@ -691,7 +725,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
@@ -708,7 +745,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
       <c r="B13">
         <v>1</v>
       </c>
@@ -725,7 +765,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
       <c r="B14">
         <v>1</v>
       </c>
@@ -742,7 +785,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
       <c r="B15">
         <v>1</v>
       </c>
@@ -759,7 +805,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
       <c r="B16">
         <v>1</v>
       </c>
@@ -776,7 +825,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
       <c r="B17">
         <v>1</v>
       </c>
@@ -793,7 +845,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
       <c r="B18">
         <v>1</v>
       </c>
@@ -810,7 +865,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
       <c r="B19">
         <v>1</v>
       </c>
@@ -827,7 +885,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
       <c r="B20">
         <v>1</v>
       </c>
@@ -844,7 +905,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
@@ -861,7 +925,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
       <c r="B22">
         <v>2</v>
       </c>
@@ -878,7 +945,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
       <c r="B23">
         <v>2</v>
       </c>
@@ -895,7 +965,10 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
       <c r="B24">
         <v>2</v>
       </c>
@@ -912,7 +985,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
       <c r="B25">
         <v>2</v>
       </c>
@@ -929,7 +1005,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
       <c r="B26">
         <v>2</v>
       </c>
@@ -946,7 +1025,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
       <c r="B27">
         <v>2</v>
       </c>
@@ -963,7 +1045,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
       <c r="B28">
         <v>2</v>
       </c>
@@ -980,7 +1065,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
       <c r="B29">
         <v>2</v>
       </c>
@@ -1000,5 +1088,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>